<commit_message>
completo para digits database (func)
</commit_message>
<xml_diff>
--- a/output/comparacao-modelos/comparacao_estrategias.xlsx
+++ b/output/comparacao-modelos/comparacao_estrategias.xlsx
@@ -8,21 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patricia/Documents/code/python-code/behavior-detection/output/comparacao-modelos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B68D95A-FB7C-144D-954B-F989423A5DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6582A864-118B-B34F-9815-72B89B0D6552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="1300" windowWidth="31160" windowHeight="17860" activeTab="3" xr2:uid="{F8066375-428B-074A-A643-CDBCF2547612}"/>
+    <workbookView xWindow="25240" yWindow="500" windowWidth="23440" windowHeight="17860" activeTab="1" xr2:uid="{F8066375-428B-074A-A643-CDBCF2547612}"/>
   </bookViews>
   <sheets>
-    <sheet name="optuna" sheetId="2" r:id="rId1"/>
-    <sheet name="skopt" sheetId="3" r:id="rId2"/>
-    <sheet name="grid" sheetId="5" r:id="rId3"/>
-    <sheet name="random" sheetId="6" r:id="rId4"/>
+    <sheet name="optuna (1)" sheetId="2" r:id="rId1"/>
+    <sheet name="optuna (2)" sheetId="8" r:id="rId2"/>
+    <sheet name="skopt" sheetId="3" r:id="rId3"/>
+    <sheet name="grid" sheetId="5" r:id="rId4"/>
+    <sheet name="random" sheetId="6" r:id="rId5"/>
+    <sheet name="comparação" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_GridSearch_avg_metrics_report_20241025_2039" localSheetId="2">grid!$A$1:$J$61</definedName>
-    <definedName name="_Optuna_avg_metrics_report_20241024_1341" localSheetId="0">optuna!$A$1:$J$36</definedName>
-    <definedName name="_RandomSearch_avg_metrics_report_20241025_2119" localSheetId="3">random!$A$1:$J$61</definedName>
-    <definedName name="_Skopt_avg_metrics_report_20241024_2203" localSheetId="1">skopt!$A$1:$J$61</definedName>
+    <definedName name="_GridSearch_avg_metrics_report_20241025_2039" localSheetId="3">grid!$A$1:$J$61</definedName>
+    <definedName name="_Optuna_avg_metrics_report_20241024_1341" localSheetId="0">'optuna (1)'!$A$1:$J$36</definedName>
+    <definedName name="_Optuna_avg_metrics_report_20241027_1826_1" localSheetId="1">'optuna (2)'!$A$1:$J$61</definedName>
+    <definedName name="_RandomSearch_avg_metrics_report_20241025_2119" localSheetId="4">random!$A$1:$J$61</definedName>
+    <definedName name="_Skopt_avg_metrics_report_20241024_2203" localSheetId="2">skopt!$A$1:$J$61</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -78,7 +81,23 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" xr16:uid="{09A50848-CB3B-7448-A60C-4FDD657DB41C}" name="_RandomSearch_avg_metrics_report_20241025_2119" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="3" xr16:uid="{B4CB4D33-6E08-2047-BFEC-BE38DFFE38C8}" name="_Optuna_avg_metrics_report_20241027_1826" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/patricia/Documents/code/python-code/behavior-detection/output/_Optuna_avg_metrics_report_20241027_1826.csv" decimal="," thousands="." semicolon="1">
+      <textFields count="10">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" xr16:uid="{09A50848-CB3B-7448-A60C-4FDD657DB41C}" name="_RandomSearch_avg_metrics_report_20241025_2119" type="6" refreshedVersion="8" background="1" saveData="1">
     <textPr codePage="10000" sourceFile="/Users/patricia/Documents/code/python-code/behavior-detection/output/comparacao-modelos/_RandomSearch_avg_metrics_report_20241025_2119.csv" decimal="," thousands="." comma="1">
       <textFields count="10">
         <textField/>
@@ -94,7 +113,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" xr16:uid="{F786EF2B-5E74-2745-A4CB-CE7D092AFCD6}" name="_Skopt_avg_metrics_report_20241024_2203" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="5" xr16:uid="{F786EF2B-5E74-2745-A4CB-CE7D092AFCD6}" name="_Skopt_avg_metrics_report_20241024_2203" type="6" refreshedVersion="8" background="1" saveData="1">
     <textPr codePage="10000" sourceFile="/Users/patricia/Documents/code/python-code/behavior-detection/output/comparacao-modelos/_Skopt_avg_metrics_report_20241024_2203.csv" decimal="," thousands="." comma="1">
       <textFields count="10">
         <textField/>
@@ -114,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="35">
   <si>
     <t>Metric</t>
   </si>
@@ -196,6 +215,30 @@
   <si>
     <t>XGBoost_pca</t>
   </si>
+  <si>
+    <t>optuna</t>
+  </si>
+  <si>
+    <t>skopt</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>grid</t>
+  </si>
+  <si>
+    <t>Modelo</t>
+  </si>
+  <si>
+    <t>Estratégia</t>
+  </si>
+  <si>
+    <t>Acurácia balanceada</t>
+  </si>
+  <si>
+    <t>Tempo (horas)</t>
+  </si>
 </sst>
 </file>
 
@@ -204,7 +247,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -225,8 +268,14 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,6 +291,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -288,21 +343,17 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -371,15 +422,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_Skopt_avg_metrics_report_20241024_2203" connectionId="4" xr16:uid="{F39CDB46-2A87-CA4A-8CD6-96536E358EFB}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_Optuna_avg_metrics_report_20241027_1826_1" connectionId="3" xr16:uid="{3763FAA5-446D-7C42-A4F8-5C1DF5385051}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_Skopt_avg_metrics_report_20241024_2203" connectionId="5" xr16:uid="{F39CDB46-2A87-CA4A-8CD6-96536E358EFB}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_GridSearch_avg_metrics_report_20241025_2039" connectionId="1" xr16:uid="{94136F04-B641-F44E-8996-4DC6B88DAC11}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_RandomSearch_avg_metrics_report_20241025_2119" connectionId="3" xr16:uid="{B188DFC7-C404-8442-891F-3987F939F15D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="_RandomSearch_avg_metrics_report_20241025_2119" connectionId="4" xr16:uid="{B188DFC7-C404-8442-891F-3987F939F15D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -702,7 +757,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="F27" sqref="F27:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1702,18 +1757,1726 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2 F7 F12 F22 F27 F32">
-    <cfRule type="top10" dxfId="3" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="4" priority="1" rank="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F15AEE-0B66-AB4C-BE44-2BB338479ED5}">
+  <dimension ref="A1:J61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12">
+        <v>0.80980618477312705</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12">
+        <v>0.78970336835413601</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="12">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0.81111111111111101</v>
+      </c>
+      <c r="G4" s="12">
+        <v>0.81111111111111101</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0.81111111111111101</v>
+      </c>
+      <c r="I4" s="12">
+        <v>0.81111111111111101</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="12">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12">
+        <v>1</v>
+      </c>
+      <c r="D5" s="12">
+        <v>1</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0.80838630474417195</v>
+      </c>
+      <c r="G5" s="12">
+        <v>0.80968134128263303</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0.80980618477312705</v>
+      </c>
+      <c r="I5" s="12">
+        <v>360</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="12">
+        <v>1</v>
+      </c>
+      <c r="C6" s="12">
+        <v>1</v>
+      </c>
+      <c r="D6" s="12">
+        <v>1</v>
+      </c>
+      <c r="E6" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0.81326404586714596</v>
+      </c>
+      <c r="G6" s="12">
+        <v>0.81842839316014804</v>
+      </c>
+      <c r="H6" s="12">
+        <v>0.81111111111111101</v>
+      </c>
+      <c r="I6" s="12">
+        <v>360</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="12">
+        <v>0.97597815152454304</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12">
+        <v>0.86648114102255103</v>
+      </c>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="12">
+        <v>0.97370471870539599</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12">
+        <v>0.85455545717895998</v>
+      </c>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="12">
+        <v>0.97633959638135004</v>
+      </c>
+      <c r="C9" s="12">
+        <v>0.97633959638135004</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0.97633959638135004</v>
+      </c>
+      <c r="E9" s="12">
+        <v>0.97633959638135004</v>
+      </c>
+      <c r="F9" s="12">
+        <v>0.86944444444444402</v>
+      </c>
+      <c r="G9" s="12">
+        <v>0.86944444444444402</v>
+      </c>
+      <c r="H9" s="12">
+        <v>0.86944444444444402</v>
+      </c>
+      <c r="I9" s="12">
+        <v>0.86944444444444402</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="12">
+        <v>0.97622560999249897</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0.97700224208549902</v>
+      </c>
+      <c r="D10" s="12">
+        <v>0.97597815152454304</v>
+      </c>
+      <c r="E10" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F10" s="12">
+        <v>0.86512570420979595</v>
+      </c>
+      <c r="G10" s="12">
+        <v>0.866635913573646</v>
+      </c>
+      <c r="H10" s="12">
+        <v>0.86648114102255103</v>
+      </c>
+      <c r="I10" s="12">
+        <v>360</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="12">
+        <v>0.97633399276819599</v>
+      </c>
+      <c r="C11" s="12">
+        <v>0.97686583820336603</v>
+      </c>
+      <c r="D11" s="12">
+        <v>0.97633959638135004</v>
+      </c>
+      <c r="E11" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F11" s="12">
+        <v>0.87031795970135395</v>
+      </c>
+      <c r="G11" s="12">
+        <v>0.87357652108235695</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0.86944444444444402</v>
+      </c>
+      <c r="I11" s="12">
+        <v>360</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12">
+        <v>0.96763153617346298</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12">
+        <v>1</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12">
+        <v>0.96285468615649095</v>
+      </c>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="12">
+        <v>1</v>
+      </c>
+      <c r="C14" s="12">
+        <v>1</v>
+      </c>
+      <c r="D14" s="12">
+        <v>1</v>
+      </c>
+      <c r="E14" s="12">
+        <v>1</v>
+      </c>
+      <c r="F14" s="12">
+        <v>0.96666666666666601</v>
+      </c>
+      <c r="G14" s="12">
+        <v>0.96666666666666601</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0.96666666666666601</v>
+      </c>
+      <c r="I14" s="12">
+        <v>0.96666666666666601</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="12">
+        <v>1</v>
+      </c>
+      <c r="C15" s="12">
+        <v>1</v>
+      </c>
+      <c r="D15" s="12">
+        <v>1</v>
+      </c>
+      <c r="E15" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F15" s="12">
+        <v>0.96680656760528405</v>
+      </c>
+      <c r="G15" s="12">
+        <v>0.966827044432226</v>
+      </c>
+      <c r="H15" s="12">
+        <v>0.96763153617346298</v>
+      </c>
+      <c r="I15" s="12">
+        <v>360</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="12">
+        <v>1</v>
+      </c>
+      <c r="C16" s="12">
+        <v>1</v>
+      </c>
+      <c r="D16" s="12">
+        <v>1</v>
+      </c>
+      <c r="E16" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F16" s="12">
+        <v>0.96670819598869195</v>
+      </c>
+      <c r="G16" s="12">
+        <v>0.96758332764985</v>
+      </c>
+      <c r="H16" s="12">
+        <v>0.96666666666666601</v>
+      </c>
+      <c r="I16" s="12">
+        <v>360</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="12">
+        <v>1</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12">
+        <v>0.97482803179298705</v>
+      </c>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="12">
+        <v>1</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12">
+        <v>0.97213190896423596</v>
+      </c>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="12">
+        <v>1</v>
+      </c>
+      <c r="C19" s="12">
+        <v>1</v>
+      </c>
+      <c r="D19" s="12">
+        <v>1</v>
+      </c>
+      <c r="E19" s="12">
+        <v>1</v>
+      </c>
+      <c r="F19" s="12">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="G19" s="12">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H19" s="12">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="I19" s="12">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="12">
+        <v>1</v>
+      </c>
+      <c r="C20" s="12">
+        <v>1</v>
+      </c>
+      <c r="D20" s="12">
+        <v>1</v>
+      </c>
+      <c r="E20" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0.97510791528041296</v>
+      </c>
+      <c r="G20" s="12">
+        <v>0.97578853342793104</v>
+      </c>
+      <c r="H20" s="12">
+        <v>0.97482803179298705</v>
+      </c>
+      <c r="I20" s="12">
+        <v>360</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="12">
+        <v>1</v>
+      </c>
+      <c r="C21" s="12">
+        <v>1</v>
+      </c>
+      <c r="D21" s="12">
+        <v>1</v>
+      </c>
+      <c r="E21" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F21" s="12">
+        <v>0.97498526166183896</v>
+      </c>
+      <c r="G21" s="12">
+        <v>0.97535813292370499</v>
+      </c>
+      <c r="H21" s="12">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="I21" s="12">
+        <v>360</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="12">
+        <v>1</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12">
+        <v>0.94640214499726305</v>
+      </c>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="12">
+        <v>1</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12">
+        <v>0.94116078417878801</v>
+      </c>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="12">
+        <v>1</v>
+      </c>
+      <c r="C24" s="12">
+        <v>1</v>
+      </c>
+      <c r="D24" s="12">
+        <v>1</v>
+      </c>
+      <c r="E24" s="12">
+        <v>1</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0.94722222222222197</v>
+      </c>
+      <c r="G24" s="12">
+        <v>0.94722222222222197</v>
+      </c>
+      <c r="H24" s="12">
+        <v>0.94722222222222197</v>
+      </c>
+      <c r="I24" s="12">
+        <v>0.94722222222222197</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="12">
+        <v>1</v>
+      </c>
+      <c r="C25" s="12">
+        <v>1</v>
+      </c>
+      <c r="D25" s="12">
+        <v>1</v>
+      </c>
+      <c r="E25" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F25" s="12">
+        <v>0.94713606066519296</v>
+      </c>
+      <c r="G25" s="12">
+        <v>0.94957959150778304</v>
+      </c>
+      <c r="H25" s="12">
+        <v>0.94640214499726305</v>
+      </c>
+      <c r="I25" s="12">
+        <v>360</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="12">
+        <v>1</v>
+      </c>
+      <c r="C26" s="12">
+        <v>1</v>
+      </c>
+      <c r="D26" s="12">
+        <v>1</v>
+      </c>
+      <c r="E26" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F26" s="12">
+        <v>0.94715615968985301</v>
+      </c>
+      <c r="G26" s="12">
+        <v>0.94856552000501404</v>
+      </c>
+      <c r="H26" s="12">
+        <v>0.94722222222222197</v>
+      </c>
+      <c r="I26" s="12">
+        <v>360</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="12">
+        <v>1</v>
+      </c>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12">
+        <v>0.98253501400560195</v>
+      </c>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="12">
+        <v>1</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12">
+        <v>0.98142542652724196</v>
+      </c>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="12">
+        <v>1</v>
+      </c>
+      <c r="C29" s="12">
+        <v>1</v>
+      </c>
+      <c r="D29" s="12">
+        <v>1</v>
+      </c>
+      <c r="E29" s="12">
+        <v>1</v>
+      </c>
+      <c r="F29" s="12">
+        <v>0.98333333333333295</v>
+      </c>
+      <c r="G29" s="12">
+        <v>0.98333333333333295</v>
+      </c>
+      <c r="H29" s="12">
+        <v>0.98333333333333295</v>
+      </c>
+      <c r="I29" s="12">
+        <v>0.98333333333333295</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="12">
+        <v>1</v>
+      </c>
+      <c r="C30" s="12">
+        <v>1</v>
+      </c>
+      <c r="D30" s="12">
+        <v>1</v>
+      </c>
+      <c r="E30" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F30" s="12">
+        <v>0.98187723529014304</v>
+      </c>
+      <c r="G30" s="12">
+        <v>0.98172619047619003</v>
+      </c>
+      <c r="H30" s="12">
+        <v>0.98253501400560195</v>
+      </c>
+      <c r="I30" s="12">
+        <v>360</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="12">
+        <v>1</v>
+      </c>
+      <c r="C31" s="12">
+        <v>1</v>
+      </c>
+      <c r="D31" s="12">
+        <v>1</v>
+      </c>
+      <c r="E31" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F31" s="12">
+        <v>0.98335178390085298</v>
+      </c>
+      <c r="G31" s="12">
+        <v>0.98384093915343895</v>
+      </c>
+      <c r="H31" s="12">
+        <v>0.98333333333333295</v>
+      </c>
+      <c r="I31" s="12">
+        <v>360</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="12">
+        <v>0.98430901779056101</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12">
+        <v>0.97535833482329104</v>
+      </c>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="12">
+        <v>0.98298522307473701</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12">
+        <v>0.97214101461736802</v>
+      </c>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="12">
+        <v>0.98469032707028503</v>
+      </c>
+      <c r="C34" s="12">
+        <v>0.98469032707028503</v>
+      </c>
+      <c r="D34" s="12">
+        <v>0.98469032707028503</v>
+      </c>
+      <c r="E34" s="12">
+        <v>0.98469032707028503</v>
+      </c>
+      <c r="F34" s="12">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="G34" s="12">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H34" s="12">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="I34" s="12">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="12">
+        <v>0.98460303541273697</v>
+      </c>
+      <c r="C35" s="12">
+        <v>0.98510681839228298</v>
+      </c>
+      <c r="D35" s="12">
+        <v>0.98430901779056101</v>
+      </c>
+      <c r="E35" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F35" s="12">
+        <v>0.97425801956062896</v>
+      </c>
+      <c r="G35" s="12">
+        <v>0.97366020044396095</v>
+      </c>
+      <c r="H35" s="12">
+        <v>0.97535833482329104</v>
+      </c>
+      <c r="I35" s="12">
+        <v>360</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="12">
+        <v>0.98467935568063703</v>
+      </c>
+      <c r="C36" s="12">
+        <v>0.98488337833651396</v>
+      </c>
+      <c r="D36" s="12">
+        <v>0.98469032707028503</v>
+      </c>
+      <c r="E36" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F36" s="12">
+        <v>0.97490750662585601</v>
+      </c>
+      <c r="G36" s="12">
+        <v>0.97529219677254797</v>
+      </c>
+      <c r="H36" s="12">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="I36" s="12">
+        <v>360</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="12">
+        <v>0.99028544876699198</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12">
+        <v>0.97996617796054497</v>
+      </c>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="12">
+        <v>0.98917281676292002</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12">
+        <v>0.97832481808329397</v>
+      </c>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="12">
+        <v>0.99025748086290799</v>
+      </c>
+      <c r="C39" s="12">
+        <v>0.99025748086290799</v>
+      </c>
+      <c r="D39" s="12">
+        <v>0.99025748086290799</v>
+      </c>
+      <c r="E39" s="12">
+        <v>0.99025748086290799</v>
+      </c>
+      <c r="F39" s="12">
+        <v>0.98055555555555496</v>
+      </c>
+      <c r="G39" s="12">
+        <v>0.98055555555555496</v>
+      </c>
+      <c r="H39" s="12">
+        <v>0.98055555555555496</v>
+      </c>
+      <c r="I39" s="12">
+        <v>0.98055555555555496</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="12">
+        <v>0.99043184910408999</v>
+      </c>
+      <c r="C40" s="12">
+        <v>0.99070210926282898</v>
+      </c>
+      <c r="D40" s="12">
+        <v>0.99028544876699198</v>
+      </c>
+      <c r="E40" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F40" s="12">
+        <v>0.98035604948157895</v>
+      </c>
+      <c r="G40" s="12">
+        <v>0.98114556167294498</v>
+      </c>
+      <c r="H40" s="12">
+        <v>0.97996617796054497</v>
+      </c>
+      <c r="I40" s="12">
+        <v>360</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" s="12">
+        <v>0.99026498050033096</v>
+      </c>
+      <c r="C41" s="12">
+        <v>0.990401314900756</v>
+      </c>
+      <c r="D41" s="12">
+        <v>0.99025748086290799</v>
+      </c>
+      <c r="E41" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F41" s="12">
+        <v>0.9805279962358</v>
+      </c>
+      <c r="G41" s="12">
+        <v>0.98084878108331397</v>
+      </c>
+      <c r="H41" s="12">
+        <v>0.98055555555555496</v>
+      </c>
+      <c r="I41" s="12">
+        <v>360</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="12">
+        <v>1</v>
+      </c>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12">
+        <v>0.97319566124321999</v>
+      </c>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="12">
+        <v>1</v>
+      </c>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12">
+        <v>0.96904663640115496</v>
+      </c>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="12">
+        <v>1</v>
+      </c>
+      <c r="C44" s="12">
+        <v>1</v>
+      </c>
+      <c r="D44" s="12">
+        <v>1</v>
+      </c>
+      <c r="E44" s="12">
+        <v>1</v>
+      </c>
+      <c r="F44" s="12">
+        <v>0.97222222222222199</v>
+      </c>
+      <c r="G44" s="12">
+        <v>0.97222222222222199</v>
+      </c>
+      <c r="H44" s="12">
+        <v>0.97222222222222199</v>
+      </c>
+      <c r="I44" s="12">
+        <v>0.97222222222222199</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" s="12">
+        <v>1</v>
+      </c>
+      <c r="C45" s="12">
+        <v>1</v>
+      </c>
+      <c r="D45" s="12">
+        <v>1</v>
+      </c>
+      <c r="E45" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F45" s="12">
+        <v>0.97201077401246505</v>
+      </c>
+      <c r="G45" s="12">
+        <v>0.97129196090440695</v>
+      </c>
+      <c r="H45" s="12">
+        <v>0.97319566124321999</v>
+      </c>
+      <c r="I45" s="12">
+        <v>360</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46" s="12">
+        <v>1</v>
+      </c>
+      <c r="C46" s="12">
+        <v>1</v>
+      </c>
+      <c r="D46" s="12">
+        <v>1</v>
+      </c>
+      <c r="E46" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F46" s="12">
+        <v>0.97201875030571305</v>
+      </c>
+      <c r="G46" s="12">
+        <v>0.97226405889926104</v>
+      </c>
+      <c r="H46" s="12">
+        <v>0.97222222222222199</v>
+      </c>
+      <c r="I46" s="12">
+        <v>360</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="12">
+        <v>1</v>
+      </c>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12">
+        <v>0.981136837713809</v>
+      </c>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="12">
+        <v>1</v>
+      </c>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12">
+        <v>0.97833040965844598</v>
+      </c>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="12">
+        <v>1</v>
+      </c>
+      <c r="C49" s="12">
+        <v>1</v>
+      </c>
+      <c r="D49" s="12">
+        <v>1</v>
+      </c>
+      <c r="E49" s="12">
+        <v>1</v>
+      </c>
+      <c r="F49" s="12">
+        <v>0.98055555555555496</v>
+      </c>
+      <c r="G49" s="12">
+        <v>0.98055555555555496</v>
+      </c>
+      <c r="H49" s="12">
+        <v>0.98055555555555496</v>
+      </c>
+      <c r="I49" s="12">
+        <v>0.98055555555555496</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" s="12">
+        <v>1</v>
+      </c>
+      <c r="C50" s="12">
+        <v>1</v>
+      </c>
+      <c r="D50" s="12">
+        <v>1</v>
+      </c>
+      <c r="E50" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F50" s="12">
+        <v>0.98052737844427196</v>
+      </c>
+      <c r="G50" s="12">
+        <v>0.98052449965493405</v>
+      </c>
+      <c r="H50" s="12">
+        <v>0.981136837713809</v>
+      </c>
+      <c r="I50" s="12">
+        <v>360</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="12">
+        <v>1</v>
+      </c>
+      <c r="C51" s="12">
+        <v>1</v>
+      </c>
+      <c r="D51" s="12">
+        <v>1</v>
+      </c>
+      <c r="E51" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F51" s="12">
+        <v>0.98052971364307595</v>
+      </c>
+      <c r="G51" s="12">
+        <v>0.98102206502568801</v>
+      </c>
+      <c r="H51" s="12">
+        <v>0.98055555555555496</v>
+      </c>
+      <c r="I51" s="12">
+        <v>360</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="12">
+        <v>1</v>
+      </c>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12">
+        <v>0.95472465581977395</v>
+      </c>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="12">
+        <v>1</v>
+      </c>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12">
+        <v>0.95046567426021</v>
+      </c>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
+      <c r="J53" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="12">
+        <v>1</v>
+      </c>
+      <c r="C54" s="12">
+        <v>1</v>
+      </c>
+      <c r="D54" s="12">
+        <v>1</v>
+      </c>
+      <c r="E54" s="12">
+        <v>1</v>
+      </c>
+      <c r="F54" s="12">
+        <v>0.95555555555555505</v>
+      </c>
+      <c r="G54" s="12">
+        <v>0.95555555555555505</v>
+      </c>
+      <c r="H54" s="12">
+        <v>0.95555555555555505</v>
+      </c>
+      <c r="I54" s="12">
+        <v>0.95555555555555505</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="12">
+        <v>1</v>
+      </c>
+      <c r="C55" s="12">
+        <v>1</v>
+      </c>
+      <c r="D55" s="12">
+        <v>1</v>
+      </c>
+      <c r="E55" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F55" s="12">
+        <v>0.95447742413121905</v>
+      </c>
+      <c r="G55" s="12">
+        <v>0.95495982314047101</v>
+      </c>
+      <c r="H55" s="12">
+        <v>0.95472465581977395</v>
+      </c>
+      <c r="I55" s="12">
+        <v>360</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B56" s="12">
+        <v>1</v>
+      </c>
+      <c r="C56" s="12">
+        <v>1</v>
+      </c>
+      <c r="D56" s="12">
+        <v>1</v>
+      </c>
+      <c r="E56" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F56" s="12">
+        <v>0.95547457193177698</v>
+      </c>
+      <c r="G56" s="12">
+        <v>0.95607804599323398</v>
+      </c>
+      <c r="H56" s="12">
+        <v>0.95555555555555505</v>
+      </c>
+      <c r="I56" s="12">
+        <v>360</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" s="12">
+        <v>1</v>
+      </c>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12">
+        <v>0.96100264965123205</v>
+      </c>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="12">
+        <v>1</v>
+      </c>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12">
+        <v>0.95665522846306605</v>
+      </c>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="12">
+        <v>1</v>
+      </c>
+      <c r="C59" s="12">
+        <v>1</v>
+      </c>
+      <c r="D59" s="12">
+        <v>1</v>
+      </c>
+      <c r="E59" s="12">
+        <v>1</v>
+      </c>
+      <c r="F59" s="12">
+        <v>0.96111111111111103</v>
+      </c>
+      <c r="G59" s="12">
+        <v>0.96111111111111103</v>
+      </c>
+      <c r="H59" s="12">
+        <v>0.96111111111111103</v>
+      </c>
+      <c r="I59" s="12">
+        <v>0.96111111111111103</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60" s="12">
+        <v>1</v>
+      </c>
+      <c r="C60" s="12">
+        <v>1</v>
+      </c>
+      <c r="D60" s="12">
+        <v>1</v>
+      </c>
+      <c r="E60" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F60" s="12">
+        <v>0.96073919028520804</v>
+      </c>
+      <c r="G60" s="12">
+        <v>0.96134665369267103</v>
+      </c>
+      <c r="H60" s="12">
+        <v>0.96100264965123205</v>
+      </c>
+      <c r="I60" s="12">
+        <v>360</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" s="12">
+        <v>1</v>
+      </c>
+      <c r="C61" s="12">
+        <v>1</v>
+      </c>
+      <c r="D61" s="12">
+        <v>1</v>
+      </c>
+      <c r="E61" s="12">
+        <v>1437</v>
+      </c>
+      <c r="F61" s="12">
+        <v>0.96117282987934205</v>
+      </c>
+      <c r="G61" s="12">
+        <v>0.961976633766224</v>
+      </c>
+      <c r="H61" s="12">
+        <v>0.96111111111111103</v>
+      </c>
+      <c r="I61" s="12">
+        <v>360</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F2 F7 F12 F17 F22 F27 F32 F37 F42 F47 F52 F57">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="5"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD155169-9248-3F4A-BDE3-FA7358CC0182}">
   <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F37" sqref="F37:J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3883,18 +5646,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2 F7 F12 F16 F22 F27 F32 F37 F42 F47 F52 F57">
-    <cfRule type="top10" dxfId="2" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="3" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF8A399-420B-3143-A50A-E76351D172FB}">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="F57" activeCellId="11" sqref="F2 F7 F12 F17 F22 F27 F32 F37 F42 F47 F52 F57"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37:J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5570,18 +7333,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2 F7 F12 F17 F22 F27 F32 F37 F42 F47 F52 F57">
-    <cfRule type="top10" dxfId="1" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="2" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3BB5389-767E-F541-A04E-64FBA65882F6}">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J37" sqref="F37:J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7257,8 +9020,102 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2 F7 F12 F17 F22 F27 F32 F37 F42 F47 F52 F57">
-    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="1" priority="1" rank="1"/>
   </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4D3C04-D7CE-D443-8029-DD6A96CA4A75}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1">
+        <f>5097/60/60</f>
+        <v>1.4158333333333333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1">
+        <f>30104/60/60</f>
+        <v>8.362222222222222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1">
+        <f>2364/60/60</f>
+        <v>0.65666666666666662</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1">
+        <f>81354/60/60</f>
+        <v>22.598333333333336</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>